<commit_message>
updated the vlan details file to take data from db
</commit_message>
<xml_diff>
--- a/vlan_details.xlsx
+++ b/vlan_details.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9F60AB-3F90-46BB-BBFF-A6EB2B581F89}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B8360D-9257-4B73-B274-E45FB6CB0127}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vlan_params" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Types" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="is_dhcp">'Data Types'!$G$7:$G$8</definedName>
+    <definedName name="is_layer3">'Data Types'!$E$7:$E$8</definedName>
+    <definedName name="vlan_type">'Data Types'!$F$7:$F$8</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>vlan_id</t>
   </si>
@@ -48,9 +54,6 @@
     <t>site_id</t>
   </si>
   <si>
-    <t>access_port_add</t>
-  </si>
-  <si>
     <t>dhcp_server</t>
   </si>
   <si>
@@ -63,35 +66,41 @@
     <t>9</t>
   </si>
   <si>
-    <t>ge-0/0/0</t>
-  </si>
-  <si>
     <t>192.168.100.20</t>
   </si>
   <si>
     <t>is_dhcp</t>
   </si>
   <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>servers</t>
+  </si>
+  <si>
+    <t>bigmamaa</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>False</t>
-  </si>
-  <si>
-    <t>Servers</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>ashertest</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +108,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -116,13 +139,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -405,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,84 +613,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{DE3D4635-DCD0-4C5E-BC5B-DCEAB351C428}">
+      <formula1>is_dhcp</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{19A49634-C75B-40EC-A5F9-1F4E687E34BB}">
+      <formula1>vlan_type</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{02E03651-EFD1-4CEF-81A7-8EE8C07B6658}">
+      <formula1>is_layer3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="261" orientation="landscape" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB85D60-4707-4712-856D-7B8648D49E99}">
+  <dimension ref="E5:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="G7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
small updated in the vlan details file
</commit_message>
<xml_diff>
--- a/vlan_details.xlsx
+++ b/vlan_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B8360D-9257-4B73-B274-E45FB6CB0127}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393A60EF-FFA0-4E28-A4CA-4A54A98C7E48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vlan_params" sheetId="1" r:id="rId1"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB85D60-4707-4712-856D-7B8648D49E99}">
   <dimension ref="E5:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
small change in the excel file
</commit_message>
<xml_diff>
--- a/vlan_details.xlsx
+++ b/vlan_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393A60EF-FFA0-4E28-A4CA-4A54A98C7E48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2D05F0-5574-42F5-AC5B-6FD584C80F4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>vlan_id</t>
   </si>
@@ -73,12 +73,6 @@
   </si>
   <si>
     <t>30</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>users</t>
@@ -603,7 +597,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +643,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -681,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -730,24 +724,24 @@
     </row>
     <row r="7" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.25">

</xml_diff>